<commit_message>
Ultimo commit del la conexion
</commit_message>
<xml_diff>
--- a/excel/patrones.xlsx
+++ b/excel/patrones.xlsx
@@ -528,13 +528,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>1000000</v>
+        <v>100000</v>
       </c>
       <c r="C7" s="5">
-        <v>147</v>
+        <v>400</v>
       </c>
       <c r="E7" s="5">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>